<commit_message>
add english sanky plot
</commit_message>
<xml_diff>
--- a/output/table/Table_1_summary_statistics.xlsx
+++ b/output/table/Table_1_summary_statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>year</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>涵蓋所有傳染途徑之週比例(%)</t>
+  </si>
+  <si>
+    <t>包含公衛衛教措施比例(%)</t>
   </si>
 </sst>
 </file>
@@ -404,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +447,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -482,8 +488,11 @@
       <c r="L2">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -520,8 +529,11 @@
       <c r="L3">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -558,8 +570,11 @@
       <c r="L4">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -596,8 +611,11 @@
       <c r="L5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -634,8 +652,11 @@
       <c r="L6">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -672,8 +693,11 @@
       <c r="L7">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -710,8 +734,11 @@
       <c r="L8">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -748,8 +775,11 @@
       <c r="L9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -786,8 +816,11 @@
       <c r="L10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -824,8 +857,11 @@
       <c r="L11">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -862,8 +898,11 @@
       <c r="L12">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -900,8 +939,11 @@
       <c r="L13">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -938,8 +980,11 @@
       <c r="L14">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -976,8 +1021,11 @@
       <c r="L15">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1014,8 +1062,11 @@
       <c r="L16">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1052,8 +1103,11 @@
       <c r="L17">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1089,6 +1143,9 @@
       </c>
       <c r="L18">
         <v>74</v>
+      </c>
+      <c r="M18">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update plots: for 初稿
</commit_message>
<xml_diff>
--- a/output/table/Table_1_summary_statistics.xlsx
+++ b/output/table/Table_1_summary_statistics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>year</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>資料來源數(不重複)</t>
-  </si>
-  <si>
-    <t>涵蓋所有傳染途徑之週比例(%)</t>
   </si>
   <si>
     <t>包含公衛防治措施比例(%)</t>
@@ -407,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,11 +444,8 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -486,13 +480,10 @@
         <v>249</v>
       </c>
       <c r="L2">
-        <v>53</v>
-      </c>
-      <c r="M2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -527,13 +518,10 @@
         <v>227</v>
       </c>
       <c r="L3">
-        <v>77</v>
-      </c>
-      <c r="M3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -568,13 +556,10 @@
         <v>192</v>
       </c>
       <c r="L4">
-        <v>85</v>
-      </c>
-      <c r="M4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -609,13 +594,10 @@
         <v>264</v>
       </c>
       <c r="L5">
-        <v>90</v>
-      </c>
-      <c r="M5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -650,13 +632,10 @@
         <v>481</v>
       </c>
       <c r="L6">
-        <v>78</v>
-      </c>
-      <c r="M6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -691,13 +670,10 @@
         <v>687</v>
       </c>
       <c r="L7">
-        <v>94</v>
-      </c>
-      <c r="M7">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -732,13 +708,10 @@
         <v>884</v>
       </c>
       <c r="L8">
-        <v>64</v>
-      </c>
-      <c r="M8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -773,13 +746,10 @@
         <v>771</v>
       </c>
       <c r="L9">
-        <v>35</v>
-      </c>
-      <c r="M9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -814,13 +784,10 @@
         <v>600</v>
       </c>
       <c r="L10">
-        <v>60</v>
-      </c>
-      <c r="M10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -855,13 +822,10 @@
         <v>426</v>
       </c>
       <c r="L11">
-        <v>83</v>
-      </c>
-      <c r="M11">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -896,13 +860,10 @@
         <v>526</v>
       </c>
       <c r="L12">
-        <v>94</v>
-      </c>
-      <c r="M12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -937,13 +898,10 @@
         <v>193</v>
       </c>
       <c r="L13">
-        <v>83</v>
-      </c>
-      <c r="M13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -978,13 +936,10 @@
         <v>146</v>
       </c>
       <c r="L14">
-        <v>88</v>
-      </c>
-      <c r="M14">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1019,13 +974,10 @@
         <v>278</v>
       </c>
       <c r="L15">
-        <v>88</v>
-      </c>
-      <c r="M15">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1060,13 +1012,10 @@
         <v>490</v>
       </c>
       <c r="L16">
-        <v>84</v>
-      </c>
-      <c r="M16">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1101,13 +1050,10 @@
         <v>1052</v>
       </c>
       <c r="L17">
-        <v>90</v>
-      </c>
-      <c r="M17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1142,9 +1088,6 @@
         <v>381</v>
       </c>
       <c r="L18">
-        <v>74</v>
-      </c>
-      <c r="M18">
         <v>34</v>
       </c>
     </row>

</xml_diff>